<commit_message>
Added COC, CZC and XOR instructions
</commit_message>
<xml_diff>
--- a/fpga/src/tms9900instructions.xlsx
+++ b/fpga/src/tms9900instructions.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/perik/Dropbox/Omat/trunk/EP994A/fpga/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epiehl/Dropbox/Omat/trunk/EP994A/fpga/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="460" windowWidth="20540" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="2320" yWindow="460" windowWidth="20540" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="82">
   <si>
     <t>A</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>Untested, does not idle</t>
-  </si>
-  <si>
-    <t>Untested, does not set ST</t>
   </si>
 </sst>
 </file>
@@ -660,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,11 +669,11 @@
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="S1">
         <f>COUNTIF(S3:S71,"&lt;&gt;")</f>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="T1">
         <f>COUNTIF(T3:T71,"&lt;&gt;")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U1" t="s">
         <v>80</v>
@@ -1265,8 +1262,8 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
-      <c r="T15" t="s">
-        <v>22</v>
+      <c r="S15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -1307,8 +1304,8 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
-      <c r="T16" t="s">
-        <v>22</v>
+      <c r="S16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -1349,8 +1346,8 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
-      <c r="T17" t="s">
-        <v>22</v>
+      <c r="S17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -2747,7 +2744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2831,7 +2828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2873,7 +2870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2915,7 +2912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2959,7 +2956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -3003,7 +3000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -3047,7 +3044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -3091,7 +3088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3141,7 +3138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -3191,7 +3188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3241,7 +3238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3291,7 +3288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3341,7 +3338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -3391,7 +3388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -3490,9 +3487,6 @@
       <c r="S64" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U64" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
@@ -3542,9 +3536,6 @@
       <c r="Q65" s="6"/>
       <c r="S65" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="U65" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
@@ -3701,9 +3692,6 @@
       <c r="S68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U68" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -3752,9 +3740,6 @@
       <c r="S69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U69" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -3803,9 +3788,6 @@
       <c r="S70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U70" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -3854,9 +3836,6 @@
       <c r="S71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U71" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B72" s="5">
@@ -3922,66 +3901,70 @@
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="M67:Q67"/>
+    <mergeCell ref="M68:Q68"/>
+    <mergeCell ref="M69:Q69"/>
+    <mergeCell ref="M70:Q70"/>
+    <mergeCell ref="M71:Q71"/>
+    <mergeCell ref="N62:Q62"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="N57:Q57"/>
+    <mergeCell ref="N58:Q58"/>
+    <mergeCell ref="N59:Q59"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="N53:Q53"/>
+    <mergeCell ref="N54:Q54"/>
+    <mergeCell ref="N55:Q55"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="J50:Q50"/>
+    <mergeCell ref="J51:Q51"/>
+    <mergeCell ref="J52:Q52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J45:Q45"/>
+    <mergeCell ref="J46:Q46"/>
+    <mergeCell ref="J47:Q47"/>
+    <mergeCell ref="J48:Q48"/>
+    <mergeCell ref="J49:Q49"/>
+    <mergeCell ref="J40:Q40"/>
+    <mergeCell ref="J41:Q41"/>
+    <mergeCell ref="J42:Q42"/>
+    <mergeCell ref="J43:Q43"/>
+    <mergeCell ref="J44:Q44"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="J37:Q37"/>
+    <mergeCell ref="J38:Q38"/>
+    <mergeCell ref="J39:Q39"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:Q27"/>
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="N22:Q22"/>
     <mergeCell ref="L23:M23"/>
@@ -3996,70 +3979,66 @@
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:Q31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="J40:Q40"/>
-    <mergeCell ref="J41:Q41"/>
-    <mergeCell ref="J42:Q42"/>
-    <mergeCell ref="J43:Q43"/>
-    <mergeCell ref="J44:Q44"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="J37:Q37"/>
-    <mergeCell ref="J38:Q38"/>
-    <mergeCell ref="J39:Q39"/>
-    <mergeCell ref="J50:Q50"/>
-    <mergeCell ref="J51:Q51"/>
-    <mergeCell ref="J52:Q52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J45:Q45"/>
-    <mergeCell ref="J46:Q46"/>
-    <mergeCell ref="J47:Q47"/>
-    <mergeCell ref="J48:Q48"/>
-    <mergeCell ref="J49:Q49"/>
-    <mergeCell ref="N57:Q57"/>
-    <mergeCell ref="N58:Q58"/>
-    <mergeCell ref="N59:Q59"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="N53:Q53"/>
-    <mergeCell ref="N54:Q54"/>
-    <mergeCell ref="N55:Q55"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="M67:Q67"/>
-    <mergeCell ref="M68:Q68"/>
-    <mergeCell ref="M69:Q69"/>
-    <mergeCell ref="M70:Q70"/>
-    <mergeCell ref="M71:Q71"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>